<commit_message>
Update June 06 2025
1. Modify plot var function to provide an output (axes).

2. Formatting in the main script
</commit_message>
<xml_diff>
--- a/BDKi_Campaigns_Info.xlsx
+++ b/BDKi_Campaigns_Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VILLAV16\Pfizer\Github\pcmm_pat_matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C1AAFB-733D-42EB-BBAB-84CA0740B8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B502BA-879F-42CF-A4C0-EAD38BB18F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26595" yWindow="5805" windowWidth="23040" windowHeight="12120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -448,7 +448,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,7 +569,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -603,7 +603,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,7 +702,7 @@
         <v>45761.770833333336</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -719,7 +719,7 @@
         <v>45764.875</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -736,7 +736,7 @@
         <v>45765.479166666664</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -899,28 +899,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f529abdc-f521-4ebe-9fd3-7c1c3e5d4c9a" xsi:nil="true"/>
-    <Presenters xmlns="9c0b11e3-08fd-4702-a1dc-460e952d9d4d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c0b11e3-08fd-4702-a1dc-460e952d9d4d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Topic xmlns="9c0b11e3-08fd-4702-a1dc-460e952d9d4d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005D4ECAFCEA7BEF4D9D3C9A4EF8E453E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31f676ab2452490776a33aaf80d5e8a3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c0b11e3-08fd-4702-a1dc-460e952d9d4d" xmlns:ns3="f529abdc-f521-4ebe-9fd3-7c1c3e5d4c9a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e1650282bbe0e64eb8f98bc9aa1a097" ns2:_="" ns3:_="">
     <xsd:import namespace="9c0b11e3-08fd-4702-a1dc-460e952d9d4d"/>
@@ -1171,10 +1149,43 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f529abdc-f521-4ebe-9fd3-7c1c3e5d4c9a" xsi:nil="true"/>
+    <Presenters xmlns="9c0b11e3-08fd-4702-a1dc-460e952d9d4d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c0b11e3-08fd-4702-a1dc-460e952d9d4d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Topic xmlns="9c0b11e3-08fd-4702-a1dc-460e952d9d4d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35157773-195C-4E4A-BA84-8CCD504DA658}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55B74965-8151-4DF2-A03F-7E04DD6DC930}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c0b11e3-08fd-4702-a1dc-460e952d9d4d"/>
+    <ds:schemaRef ds:uri="f529abdc-f521-4ebe-9fd3-7c1c3e5d4c9a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1191,20 +1202,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55B74965-8151-4DF2-A03F-7E04DD6DC930}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35157773-195C-4E4A-BA84-8CCD504DA658}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9c0b11e3-08fd-4702-a1dc-460e952d9d4d"/>
-    <ds:schemaRef ds:uri="f529abdc-f521-4ebe-9fd3-7c1c3e5d4c9a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>